<commit_message>
[feat] enhance CTASection on landing page; add feature highlights with icons and descriptions, update layout for improved user engagement
</commit_message>
<xml_diff>
--- a/frontend/public/example.xlsx
+++ b/frontend/public/example.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,220 +446,2200 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>common.hello</t>
+          <t>common.title.create_0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hello</t>
+          <t>English text for common title create item 0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>안녕하세요</t>
+          <t>common title create 항목 0의 한국어 텍스트</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>こんにちは</t>
+          <t>common title create アイテム 0 の日本語テキスト</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>common.goodbye</t>
+          <t>auth.title.create_1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Goodbye</t>
+          <t>English text for auth title create item 1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>안녕히 가세요</t>
+          <t>auth title create 항목 1의 한국어 텍스트</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>さようなら</t>
+          <t>auth title create アイテム 1 の日本語テキスト</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>common.welcome</t>
+          <t>dashboard.title.create_2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Welcome</t>
+          <t>English text for dashboard title create item 2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>환영합니다</t>
+          <t>dashboard title create 항목 2의 한국어 텍스트</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ようこそ</t>
+          <t>dashboard title create アイテム 2 の日本語テキスト</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>common.thanks</t>
+          <t>settings.title.create_3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Thank you</t>
+          <t>English text for settings title create item 3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>감사합니다</t>
+          <t>settings title create 항목 3의 한국어 텍스트</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ありがとう</t>
+          <t>settings title create アイテム 3 の日本語テキスト</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>common.yes</t>
+          <t>profile.title.create_4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>English text for profile title create item 4</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>예</t>
+          <t>profile title create 항목 4의 한국어 텍스트</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>はい</t>
+          <t>profile title create アイテム 4 の日本語テキスト</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>common.no</t>
+          <t>notifications.title.create_5</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>English text for notifications title create item 5</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>아니오</t>
+          <t>notifications title create 항목 5의 한국어 텍스트</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>いいえ</t>
+          <t>notifications title create アイテム 5 の日本語テキスト</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>common.ok</t>
+          <t>messages.title.create_6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>English text for messages title create item 6</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>확인</t>
+          <t>messages title create 항목 6의 한국어 텍스트</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>messages title create アイテム 6 の日本語テキスト</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>common.cancel</t>
+          <t>errors.title.create_7</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cancel</t>
+          <t>English text for errors title create item 7</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>취소</t>
+          <t>errors title create 항목 7의 한국어 텍스트</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>キャンセル</t>
+          <t>errors title create アイテム 7 の日本語テキスト</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>common.save</t>
+          <t>validation.title.create_8</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Save</t>
+          <t>English text for validation title create item 8</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>저장</t>
+          <t>validation title create 항목 8의 한국어 텍스트</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>保存</t>
+          <t>validation title create アイテム 8 の日本語テキスト</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>common.delete</t>
+          <t>buttons.title.create_9</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Delete</t>
+          <t>English text for buttons title create item 9</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>삭제</t>
+          <t>buttons title create 항목 9의 한국어 텍스트</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>削除</t>
+          <t>buttons title create アイテム 9 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>common.description.create_10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>English text for common description create item 10</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>common description create 항목 10의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>common description create アイテム 10 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>auth.description.create_11</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>English text for auth description create item 11</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>auth description create 항목 11의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>auth description create アイテム 11 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>dashboard.description.create_12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>English text for dashboard description create item 12</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>dashboard description create 항목 12의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>dashboard description create アイテム 12 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>settings.description.create_13</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>English text for settings description create item 13</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>settings description create 항목 13의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>settings description create アイテム 13 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>profile.description.create_14</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>English text for profile description create item 14</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>profile description create 항목 14의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>profile description create アイテム 14 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>notifications.description.create_15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>English text for notifications description create item 15</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>notifications description create 항목 15의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>notifications description create アイテム 15 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>messages.description.create_16</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>English text for messages description create item 16</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>messages description create 항목 16의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>messages description create アイテム 16 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>errors.description.create_17</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>English text for errors description create item 17</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>errors description create 항목 17의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>errors description create アイテム 17 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>validation.description.create_18</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>English text for validation description create item 18</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>validation description create 항목 18의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>validation description create アイテム 18 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>buttons.description.create_19</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>English text for buttons description create item 19</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>buttons description create 항목 19의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>buttons description create アイテム 19 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>common.label.create_20</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>English text for common label create item 20</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>common label create 항목 20의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>common label create アイテム 20 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>auth.label.create_21</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>English text for auth label create item 21</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>auth label create 항목 21의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>auth label create アイテム 21 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>dashboard.label.create_22</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>English text for dashboard label create item 22</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>dashboard label create 항목 22의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>dashboard label create アイテム 22 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>settings.label.create_23</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>English text for settings label create item 23</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>settings label create 항목 23의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>settings label create アイテム 23 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>profile.label.create_24</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>English text for profile label create item 24</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>profile label create 항목 24의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>profile label create アイテム 24 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>notifications.label.create_25</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>English text for notifications label create item 25</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>notifications label create 항목 25의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>notifications label create アイテム 25 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>messages.label.create_26</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>English text for messages label create item 26</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>messages label create 항목 26의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>messages label create アイテム 26 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>errors.label.create_27</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>English text for errors label create item 27</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>errors label create 항목 27의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>errors label create アイテム 27 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>validation.label.create_28</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>English text for validation label create item 28</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>validation label create 항목 28의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>validation label create アイテム 28 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>buttons.label.create_29</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>English text for buttons label create item 29</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>buttons label create 항목 29의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>buttons label create アイテム 29 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>common.placeholder.create_30</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>English text for common placeholder create item 30</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>common placeholder create 항목 30의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>common placeholder create アイテム 30 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>auth.placeholder.create_31</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>English text for auth placeholder create item 31</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>auth placeholder create 항목 31의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>auth placeholder create アイテム 31 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>dashboard.placeholder.create_32</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>English text for dashboard placeholder create item 32</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>dashboard placeholder create 항목 32의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>dashboard placeholder create アイテム 32 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>settings.placeholder.create_33</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>English text for settings placeholder create item 33</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>settings placeholder create 항목 33의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>settings placeholder create アイテム 33 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>profile.placeholder.create_34</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>English text for profile placeholder create item 34</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>profile placeholder create 항목 34의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>profile placeholder create アイテム 34 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>notifications.placeholder.create_35</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>English text for notifications placeholder create item 35</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>notifications placeholder create 항목 35의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>notifications placeholder create アイテム 35 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>messages.placeholder.create_36</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>English text for messages placeholder create item 36</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>messages placeholder create 항목 36의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>messages placeholder create アイテム 36 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>errors.placeholder.create_37</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>English text for errors placeholder create item 37</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>errors placeholder create 항목 37의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>errors placeholder create アイテム 37 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>validation.placeholder.create_38</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>English text for validation placeholder create item 38</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>validation placeholder create 항목 38의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>validation placeholder create アイテム 38 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>buttons.placeholder.create_39</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>English text for buttons placeholder create item 39</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>buttons placeholder create 항목 39의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>buttons placeholder create アイテム 39 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>common.hint.create_40</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>English text for common hint create item 40</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>common hint create 항목 40의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>common hint create アイテム 40 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>auth.hint.create_41</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>English text for auth hint create item 41</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>auth hint create 항목 41의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>auth hint create アイテム 41 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>dashboard.hint.create_42</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>English text for dashboard hint create item 42</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>dashboard hint create 항목 42의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>dashboard hint create アイテム 42 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>settings.hint.create_43</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>English text for settings hint create item 43</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>settings hint create 항목 43의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>settings hint create アイテム 43 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>profile.hint.create_44</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>English text for profile hint create item 44</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>profile hint create 항목 44의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>profile hint create アイテム 44 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>notifications.hint.create_45</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>English text for notifications hint create item 45</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>notifications hint create 항목 45의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>notifications hint create アイテム 45 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>messages.hint.create_46</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>English text for messages hint create item 46</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>messages hint create 항목 46의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>messages hint create アイテム 46 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>errors.hint.create_47</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>English text for errors hint create item 47</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>errors hint create 항목 47의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>errors hint create アイテム 47 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>validation.hint.create_48</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>English text for validation hint create item 48</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>validation hint create 항목 48의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>validation hint create アイテム 48 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>buttons.hint.create_49</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>English text for buttons hint create item 49</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>buttons hint create 항목 49의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>buttons hint create アイテム 49 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>common.error.create_50</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>English text for common error create item 50</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>common error create 항목 50의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>common error create アイテム 50 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>auth.error.create_51</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>English text for auth error create item 51</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>auth error create 항목 51의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>auth error create アイテム 51 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>dashboard.error.create_52</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>English text for dashboard error create item 52</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>dashboard error create 항목 52의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>dashboard error create アイテム 52 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>settings.error.create_53</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>English text for settings error create item 53</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>settings error create 항목 53의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>settings error create アイテム 53 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>profile.error.create_54</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>English text for profile error create item 54</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>profile error create 항목 54의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>profile error create アイテム 54 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>notifications.error.create_55</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>English text for notifications error create item 55</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>notifications error create 항목 55의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>notifications error create アイテム 55 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>messages.error.create_56</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>English text for messages error create item 56</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>messages error create 항목 56의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>messages error create アイテム 56 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>errors.error.create_57</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>English text for errors error create item 57</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>errors error create 항목 57의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>errors error create アイテム 57 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>validation.error.create_58</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>English text for validation error create item 58</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>validation error create 항목 58의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>validation error create アイテム 58 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>buttons.error.create_59</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>English text for buttons error create item 59</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>buttons error create 항목 59의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>buttons error create アイテム 59 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>common.success.create_60</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>English text for common success create item 60</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>common success create 항목 60의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>common success create アイテム 60 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>auth.success.create_61</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>English text for auth success create item 61</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>auth success create 항목 61의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>auth success create アイテム 61 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>dashboard.success.create_62</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>English text for dashboard success create item 62</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>dashboard success create 항목 62의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>dashboard success create アイテム 62 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>settings.success.create_63</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>English text for settings success create item 63</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>settings success create 항목 63의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>settings success create アイテム 63 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>profile.success.create_64</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>English text for profile success create item 64</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>profile success create 항목 64의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>profile success create アイテム 64 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>notifications.success.create_65</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>English text for notifications success create item 65</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>notifications success create 항목 65의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>notifications success create アイテム 65 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>messages.success.create_66</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>English text for messages success create item 66</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>messages success create 항목 66의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>messages success create アイテム 66 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>errors.success.create_67</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>English text for errors success create item 67</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>errors success create 항목 67의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>errors success create アイテム 67 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>validation.success.create_68</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>English text for validation success create item 68</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>validation success create 항목 68의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>validation success create アイテム 68 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>buttons.success.create_69</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>English text for buttons success create item 69</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>buttons success create 항목 69의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>buttons success create アイテム 69 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>common.warning.create_70</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>English text for common warning create item 70</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>common warning create 항목 70의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>common warning create アイテム 70 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>auth.warning.create_71</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>English text for auth warning create item 71</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>auth warning create 항목 71의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>auth warning create アイテム 71 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>dashboard.warning.create_72</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>English text for dashboard warning create item 72</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>dashboard warning create 항목 72의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>dashboard warning create アイテム 72 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>settings.warning.create_73</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>English text for settings warning create item 73</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>settings warning create 항목 73의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>settings warning create アイテム 73 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>profile.warning.create_74</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>English text for profile warning create item 74</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>profile warning create 항목 74의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>profile warning create アイテム 74 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>notifications.warning.create_75</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>English text for notifications warning create item 75</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>notifications warning create 항목 75의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>notifications warning create アイテム 75 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>messages.warning.create_76</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>English text for messages warning create item 76</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>messages warning create 항목 76의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>messages warning create アイテム 76 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>errors.warning.create_77</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>English text for errors warning create item 77</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>errors warning create 항목 77의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>errors warning create アイテム 77 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>validation.warning.create_78</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>English text for validation warning create item 78</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>validation warning create 항목 78의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>validation warning create アイテム 78 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>buttons.warning.create_79</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>English text for buttons warning create item 79</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>buttons warning create 항목 79의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>buttons warning create アイテム 79 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>common.info.create_80</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>English text for common info create item 80</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>common info create 항목 80의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>common info create アイテム 80 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>auth.info.create_81</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>English text for auth info create item 81</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>auth info create 항목 81의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>auth info create アイテム 81 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>dashboard.info.create_82</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>English text for dashboard info create item 82</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>dashboard info create 항목 82의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>dashboard info create アイテム 82 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>settings.info.create_83</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>English text for settings info create item 83</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>settings info create 항목 83의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>settings info create アイテム 83 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>profile.info.create_84</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>English text for profile info create item 84</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>profile info create 항목 84의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>profile info create アイテム 84 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>notifications.info.create_85</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>English text for notifications info create item 85</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>notifications info create 항목 85의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>notifications info create アイテム 85 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>messages.info.create_86</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>English text for messages info create item 86</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>messages info create 항목 86의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>messages info create アイテム 86 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>errors.info.create_87</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>English text for errors info create item 87</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>errors info create 항목 87의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>errors info create アイテム 87 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>validation.info.create_88</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>English text for validation info create item 88</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>validation info create 항목 88의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>validation info create アイテム 88 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>buttons.info.create_89</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>English text for buttons info create item 89</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>buttons info create 항목 89의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>buttons info create アイテム 89 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>common.help.create_90</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>English text for common help create item 90</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>common help create 항목 90의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>common help create アイテム 90 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>auth.help.create_91</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>English text for auth help create item 91</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>auth help create 항목 91의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>auth help create アイテム 91 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>dashboard.help.create_92</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>English text for dashboard help create item 92</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>dashboard help create 항목 92의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>dashboard help create アイテム 92 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>settings.help.create_93</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>English text for settings help create item 93</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>settings help create 항목 93의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>settings help create アイテム 93 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>profile.help.create_94</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>English text for profile help create item 94</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>profile help create 항목 94의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>profile help create アイテム 94 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>notifications.help.create_95</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>English text for notifications help create item 95</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>notifications help create 항목 95의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>notifications help create アイテム 95 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>messages.help.create_96</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>English text for messages help create item 96</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>messages help create 항목 96의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>messages help create アイテム 96 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>errors.help.create_97</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>English text for errors help create item 97</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>errors help create 항목 97의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>errors help create アイテム 97 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>validation.help.create_98</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>English text for validation help create item 98</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>validation help create 항목 98의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>validation help create アイテム 98 の日本語テキスト</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>buttons.help.create_99</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>English text for buttons help create item 99</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>buttons help create 항목 99의 한국어 텍스트</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>buttons help create アイテム 99 の日本語テキスト</t>
         </is>
       </c>
     </row>

</xml_diff>